<commit_message>
Finished - code review
Finished project. Testing result = Working. Ready for code review.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndreiKrausz\Documents\GitHub\POC2_API_dogs_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C089438D-1C73-47FF-87EC-C2A8A2516FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5291C65-5BF5-4C23-8163-9DE56BAC60C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -195,6 +195,18 @@
   </si>
   <si>
     <t>Why so serious ?</t>
+  </si>
+  <si>
+    <t>Subject2</t>
+  </si>
+  <si>
+    <t>Mergem la Untold ?</t>
+  </si>
+  <si>
+    <t>MailManagers</t>
+  </si>
+  <si>
+    <t>apiDogsMailManager</t>
   </si>
 </sst>
 </file>
@@ -581,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -723,7 +735,14 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1716,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2879,8 +2898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2927,7 +2946,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>